<commit_message>
Comment and Bracket Restructure
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="125">
   <si>
     <t>Start Date</t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t>Extension: F, D, Q</t>
+  </si>
+  <si>
+    <t>Use Kate Editor icons, maybe</t>
   </si>
 </sst>
 </file>
@@ -1336,10 +1339,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7</c:v>
@@ -1384,25 +1387,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0</c:v>
@@ -1423,7 +1426,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>16</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1878,10 +1881,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>91</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1926,25 +1929,25 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>91</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>28</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>28</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>28</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>28</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>21</c:v>
@@ -1965,7 +1968,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>91</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3117,11 +3120,11 @@
       </c>
       <c r="F5" s="13">
         <f ca="1">IF(((D5)=""),"",TODAY()-C5)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G5" s="13">
         <f t="shared" ref="G5:G10" ca="1" si="0">IF(F5="","",(D5-C5)-F5)</f>
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3140,11 +3143,11 @@
       </c>
       <c r="F6" s="13">
         <f t="shared" ref="F6:F20" ca="1" si="2">IF(((D6)=""),"",IF(TODAY()&lt;C6,0,IF(TODAY()&lt;D6,TODAY()-C6,E6)))</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G6" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I6" s="4"/>
     </row>
@@ -3487,11 +3490,11 @@
       </c>
       <c r="F21" s="13">
         <f ca="1">IF(((D21)=""),"",TODAY()-C21)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G21" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3510,11 +3513,11 @@
       </c>
       <c r="F22" s="13">
         <f t="shared" ref="F22:F33" ca="1" si="6">IF(((D22)=""),"",IF(TODAY()&lt;C22,0,IF(TODAY()&lt;D22,TODAY()-C22,E22)))</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G22" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3533,11 +3536,11 @@
       </c>
       <c r="F23" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G23" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3556,11 +3559,11 @@
       </c>
       <c r="F24" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="13">
         <f t="shared" ref="G24:G27" ca="1" si="7">IF(F24="","",(D24-C24)-F24)</f>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3579,11 +3582,11 @@
       </c>
       <c r="F25" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="13">
         <f t="shared" ca="1" si="7"/>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3602,11 +3605,11 @@
       </c>
       <c r="F26" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="13">
         <f t="shared" ca="1" si="7"/>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3625,11 +3628,11 @@
       </c>
       <c r="F27" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="13">
         <f t="shared" ca="1" si="7"/>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3786,11 +3789,11 @@
       </c>
       <c r="F34" s="13">
         <f ca="1">IF(((D34)=""),"",TODAY()-C34)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G34" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3806,10 +3809,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -4192,38 +4195,43 @@
         <v>118</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A87" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="B86" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A88" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="B88" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="B89" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="C89" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="C90" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A91" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A92" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="B92" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B93" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B94" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="B95" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Save Point :: Parser
Trying JavaCC instead of writing my own.
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10284" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10284" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="130">
   <si>
     <t>Start Date</t>
   </si>
@@ -124,9 +124,6 @@
     <t>Distribution of Work</t>
   </si>
   <si>
-    <t>Interpreter</t>
-  </si>
-  <si>
     <t>Registers</t>
   </si>
   <si>
@@ -394,16 +391,34 @@
     <t>Have status bar of loading or launch count down</t>
   </si>
   <si>
-    <t>Splash, Terminal, Command/Control Bar, Sub-Menus</t>
-  </si>
-  <si>
     <t>Extension: M, N, V</t>
   </si>
   <si>
     <t>Extension: F, D, Q</t>
   </si>
   <si>
-    <t>Use Kate Editor icons, maybe</t>
+    <t>Splash and GUI</t>
+  </si>
+  <si>
+    <t>Sub-Menu</t>
+  </si>
+  <si>
+    <t>Octal display</t>
+  </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <t>Open source icon</t>
+  </si>
+  <si>
+    <t>Vectorized icons if possible</t>
+  </si>
+  <si>
+    <t>Record where icon are taken from to proper citation</t>
+  </si>
+  <si>
+    <t>System Bar</t>
   </si>
 </sst>
 </file>
@@ -755,7 +770,7 @@
                   <c:v>Distribution of Work</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Interpreter</c:v>
+                  <c:v>Assembler</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>Memory &amp; Registers</c:v>
@@ -764,7 +779,7 @@
                   <c:v>File Editor</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Splash, Terminal, Command/Control Bar, Sub-Menus</c:v>
+                  <c:v>Splash and GUI</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>Integration &amp; Debugging</c:v>
@@ -1297,7 +1312,7 @@
                   <c:v>Distribution of Work</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Interpreter</c:v>
+                  <c:v>Assembler</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>Memory &amp; Registers</c:v>
@@ -1306,7 +1321,7 @@
                   <c:v>File Editor</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Splash, Terminal, Command/Control Bar, Sub-Menus</c:v>
+                  <c:v>Splash and GUI</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>Integration &amp; Debugging</c:v>
@@ -1339,10 +1354,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7</c:v>
@@ -1387,7 +1402,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>14</c:v>
@@ -1396,16 +1411,16 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0</c:v>
@@ -1426,7 +1441,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>20</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1839,7 +1854,7 @@
                   <c:v>Distribution of Work</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Interpreter</c:v>
+                  <c:v>Assembler</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>Memory &amp; Registers</c:v>
@@ -1848,7 +1863,7 @@
                   <c:v>File Editor</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Splash, Terminal, Command/Control Bar, Sub-Menus</c:v>
+                  <c:v>Splash and GUI</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>Integration &amp; Debugging</c:v>
@@ -1881,10 +1896,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>87</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1929,7 +1944,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>87</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -1938,16 +1953,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>27</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>27</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>27</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>27</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>21</c:v>
@@ -1968,7 +1983,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>87</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3003,14 +3018,14 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:U34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="2.6484375" customWidth="1"/>
-    <col min="2" max="2" width="43.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6484375" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12.6484375" customWidth="1"/>
     <col min="6" max="7" width="12.6484375" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="3.5" customWidth="1"/>
@@ -3120,11 +3135,11 @@
       </c>
       <c r="F5" s="13">
         <f ca="1">IF(((D5)=""),"",TODAY()-C5)</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G5" s="13">
         <f t="shared" ref="G5:G10" ca="1" si="0">IF(F5="","",(D5-C5)-F5)</f>
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3143,17 +3158,17 @@
       </c>
       <c r="F6" s="13">
         <f t="shared" ref="F6:F20" ca="1" si="2">IF(((D6)=""),"",IF(TODAY()&lt;C6,0,IF(TODAY()&lt;D6,TODAY()-C6,E6)))</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G6" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B7" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" s="3">
         <v>43125</v>
@@ -3176,7 +3191,7 @@
     </row>
     <row r="8" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B8" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="3">
         <v>43143</v>
@@ -3268,7 +3283,7 @@
     </row>
     <row r="12" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B12" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="3">
         <v>43178</v>
@@ -3490,16 +3505,16 @@
       </c>
       <c r="F21" s="13">
         <f ca="1">IF(((D21)=""),"",TODAY()-C21)</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G21" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B22" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C22" s="3">
         <v>43121</v>
@@ -3545,7 +3560,7 @@
     </row>
     <row r="24" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B24" s="14" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="C24" s="3">
         <v>43135</v>
@@ -3559,16 +3574,16 @@
       </c>
       <c r="F24" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G24" s="13">
         <f t="shared" ref="G24:G27" ca="1" si="7">IF(F24="","",(D24-C24)-F24)</f>
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B25" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" s="3">
         <v>43135</v>
@@ -3582,11 +3597,11 @@
       </c>
       <c r="F25" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G25" s="13">
         <f t="shared" ca="1" si="7"/>
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3605,16 +3620,16 @@
       </c>
       <c r="F26" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G26" s="13">
         <f t="shared" ca="1" si="7"/>
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B27" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C27" s="3">
         <v>43135</v>
@@ -3628,16 +3643,16 @@
       </c>
       <c r="F27" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G27" s="13">
         <f t="shared" ca="1" si="7"/>
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B28" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C28" s="3">
         <v>43156</v>
@@ -3660,7 +3675,7 @@
     </row>
     <row r="29" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B29" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C29" s="3">
         <v>43170</v>
@@ -3683,7 +3698,7 @@
     </row>
     <row r="30" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B30" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C30" s="3">
         <v>43170</v>
@@ -3706,7 +3721,7 @@
     </row>
     <row r="31" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B31" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C31" s="3">
         <v>43170</v>
@@ -3729,7 +3744,7 @@
     </row>
     <row r="32" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B32" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C32" s="3">
         <v>43170</v>
@@ -3789,11 +3804,11 @@
       </c>
       <c r="F34" s="13">
         <f ca="1">IF(((D34)=""),"",TODAY()-C34)</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G34" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3809,10 +3824,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -3822,42 +3837,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.6">
@@ -3867,127 +3882,127 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A38" t="s">
-        <v>33</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="B37" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="B39" t="s">
-        <v>48</v>
+      <c r="A39" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B40" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="C41" t="s">
-        <v>51</v>
+      <c r="B41" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.6">
@@ -3997,242 +4012,262 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.6">
       <c r="C43" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="B44" t="s">
-        <v>52</v>
+      <c r="C44" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.6">
       <c r="C45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="B46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="C47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="C48" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="C46" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A48" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="B49" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A50" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="B51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="C52" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="C53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="C54" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="C55" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="B56" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="C50" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="C51" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="C57" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="C52" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="C58" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="C53" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="B59" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="C60" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="C61" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="B62" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="C63" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="B54" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="C55" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="C56" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="B57" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="C58" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="C59" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="B60" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="C64" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="B65" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="C61" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="C62" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="C66" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="B63" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.6">
-      <c r="C64" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="C65" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="B66" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.6">
       <c r="C67" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="D68" t="s">
-        <v>99</v>
+      <c r="B68" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="E69" t="s">
+      <c r="C69" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="D70" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E71" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E72" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="E70" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="C71" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="D72" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="C73" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="D73" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.6">
       <c r="D74" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.6">
       <c r="D75" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="D76" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A77" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="B78" t="s">
-        <v>119</v>
+      <c r="D77" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="B79" t="s">
-        <v>109</v>
+      <c r="A79" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.6">
       <c r="B80" t="s">
-        <v>120</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="B81" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A82" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="B83" t="s">
-        <v>116</v>
+      <c r="B82" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="B84" t="s">
-        <v>117</v>
+      <c r="A84" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B85" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B86" t="s">
-        <v>124</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="B87" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A88" t="s">
-        <v>96</v>
+      <c r="B88" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="B89" t="s">
-        <v>97</v>
+      <c r="C89" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.6">
       <c r="C90" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A92" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B93" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="B94" t="s">
+      <c r="C94" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A96" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.6">
+      <c r="B97" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.6">
+      <c r="B98" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.6">
+      <c r="B99" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="B95" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -4242,7 +4277,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -4256,7 +4291,7 @@
     <col min="4" max="4" width="2.5" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
     <col min="6" max="6" width="2.5" customWidth="1"/>
-    <col min="7" max="7" width="43.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
     <col min="8" max="8" width="2.5" customWidth="1"/>
     <col min="9" max="9" width="17.5" customWidth="1"/>
     <col min="10" max="10" width="2.5" customWidth="1"/>
@@ -4289,20 +4324,35 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.6">
+      <c r="G7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.6">
+      <c r="G8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.6">
+      <c r="G9" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forgot to stage files
Files didn't stage correctly
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -1366,7 +1366,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>28</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>27</c:v>
@@ -1375,19 +1375,19 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1417,7 +1417,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>28</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>14</c:v>
@@ -1426,19 +1426,19 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
@@ -1456,7 +1456,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>28</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1914,7 +1914,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>79</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1923,19 +1923,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>7</c:v>
@@ -1965,7 +1965,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>79</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -1974,19 +1974,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>28</c:v>
@@ -2004,7 +2004,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>79</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3156,11 +3156,11 @@
       </c>
       <c r="F5" s="13">
         <f ca="1">IF(((D5)=""),"",TODAY()-C5)</f>
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="G5" s="13">
         <f t="shared" ref="G5:G11" ca="1" si="0">IF(F5="","",(D5-C5)-F5)</f>
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3226,11 +3226,11 @@
       </c>
       <c r="F8" s="13">
         <f t="shared" ref="F8" ca="1" si="3">IF(((D8)=""),"",IF(TODAY()&lt;C8,0,IF(TODAY()&lt;D8,TODAY()-C8,E8)))</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G8" s="13">
         <f t="shared" ref="G8" ca="1" si="4">IF(F8="","",(D8-C8)-F8)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3272,11 +3272,11 @@
       </c>
       <c r="F10" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G10" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3295,11 +3295,11 @@
       </c>
       <c r="F11" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G11" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3318,11 +3318,11 @@
       </c>
       <c r="F12" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G12" s="13">
         <f t="shared" ref="G12:G35" ca="1" si="6">IF(F12="","",(D12-C12)-F12)</f>
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3549,11 +3549,11 @@
       </c>
       <c r="F22" s="13">
         <f ca="1">IF(((D22)=""),"",TODAY()-C22)</f>
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="G22" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3618,11 +3618,11 @@
       </c>
       <c r="F25" s="13">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G25" s="13">
         <f t="shared" ref="G25:G28" ca="1" si="9">IF(F25="","",(D25-C25)-F25)</f>
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3641,11 +3641,11 @@
       </c>
       <c r="F26" s="13">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G26" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3664,11 +3664,11 @@
       </c>
       <c r="F27" s="13">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G27" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3687,11 +3687,11 @@
       </c>
       <c r="F28" s="13">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G28" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3710,11 +3710,11 @@
       </c>
       <c r="F29" s="13">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G29" s="13">
         <f t="shared" ref="G29:G33" ca="1" si="11">IF(F29="","",(D29-C29)-F29)</f>
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3848,11 +3848,11 @@
       </c>
       <c r="F35" s="13">
         <f ca="1">IF(((D35)=""),"",TODAY()-C35)</f>
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="G35" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Assembler is considered complete
Handles errors and correct code.
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -340,12 +340,6 @@
     <t>Integration &amp; Debugging</t>
   </si>
   <si>
-    <t>Extension: A, C</t>
-  </si>
-  <si>
-    <t>IEEE 754 Converter (Single, Double)</t>
-  </si>
-  <si>
     <t>Project Presentation 2 Deliverables</t>
   </si>
   <si>
@@ -391,12 +385,6 @@
     <t>Have status bar of loading or launch count down</t>
   </si>
   <si>
-    <t>Extension: M, N, V</t>
-  </si>
-  <si>
-    <t>Extension: F, D, Q</t>
-  </si>
-  <si>
     <t>Splash and GUI</t>
   </si>
   <si>
@@ -422,6 +410,18 @@
   </si>
   <si>
     <t>Project Abstract</t>
+  </si>
+  <si>
+    <t>Extension: Simulator</t>
+  </si>
+  <si>
+    <t>Extension: M, A, F, D</t>
+  </si>
+  <si>
+    <t>(Optional) IEEE 754 Converter (Single, Double)</t>
+  </si>
+  <si>
+    <t>(Optional)  Extension Q &amp; Help Screen</t>
   </si>
 </sst>
 </file>
@@ -791,16 +791,16 @@
                   <c:v>Integration &amp; Debugging</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Extension: M, N, V</c:v>
+                  <c:v>Extension: Simulator</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Extension: A, C</c:v>
+                  <c:v>Extension: M, A, F, D</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Extension: F, D, Q</c:v>
+                  <c:v>(Optional)  Extension Q &amp; Help Screen</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>IEEE 754 Converter (Single, Double)</c:v>
+                  <c:v>(Optional) IEEE 754 Converter (Single, Double)</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>Final Integration &amp; Debugging</c:v>
@@ -899,10 +899,10 @@
                   <c:v>43170</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43170</c:v>
+                  <c:v>43184</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43170</c:v>
+                  <c:v>43184</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>43184</c:v>
@@ -1339,16 +1339,16 @@
                   <c:v>Integration &amp; Debugging</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Extension: M, N, V</c:v>
+                  <c:v>Extension: Simulator</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Extension: A, C</c:v>
+                  <c:v>Extension: M, A, F, D</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Extension: F, D, Q</c:v>
+                  <c:v>(Optional)  Extension Q &amp; Help Screen</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>IEEE 754 Converter (Single, Double)</c:v>
+                  <c:v>(Optional) IEEE 754 Converter (Single, Double)</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>Final Integration &amp; Debugging</c:v>
@@ -1366,7 +1366,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>42</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>27</c:v>
@@ -1384,13 +1384,13 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -1417,7 +1417,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>42</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>14</c:v>
@@ -1426,25 +1426,25 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>23</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>23</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>23</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>0</c:v>
@@ -1456,7 +1456,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>42</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1887,16 +1887,16 @@
                   <c:v>Integration &amp; Debugging</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Extension: M, N, V</c:v>
+                  <c:v>Extension: Simulator</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Extension: A, C</c:v>
+                  <c:v>Extension: M, A, F, D</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Extension: F, D, Q</c:v>
+                  <c:v>(Optional)  Extension Q &amp; Help Screen</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>IEEE 754 Converter (Single, Double)</c:v>
+                  <c:v>(Optional) IEEE 754 Converter (Single, Double)</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>Final Integration &amp; Debugging</c:v>
@@ -1914,7 +1914,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>65</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1932,13 +1932,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>5</c:v>
@@ -1965,7 +1965,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>65</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -1974,37 +1974,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>19</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>28</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>28</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>65</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3039,14 +3039,14 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:U35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="2.6484375" customWidth="1"/>
-    <col min="2" max="2" width="29.6484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.34765625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12.6484375" customWidth="1"/>
     <col min="6" max="7" width="12.6484375" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="3.5" customWidth="1"/>
@@ -3156,11 +3156,11 @@
       </c>
       <c r="F5" s="13">
         <f ca="1">IF(((D5)=""),"",TODAY()-C5)</f>
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="G5" s="13">
         <f t="shared" ref="G5:G11" ca="1" si="0">IF(F5="","",(D5-C5)-F5)</f>
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3189,7 +3189,7 @@
     </row>
     <row r="7" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B7" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C7" s="3">
         <v>43125</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="8" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B8" s="14" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C8" s="3">
         <v>43140</v>
@@ -3235,7 +3235,7 @@
     </row>
     <row r="9" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B9" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C9" s="3">
         <v>43136</v>
@@ -3295,11 +3295,11 @@
       </c>
       <c r="F11" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="G11" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3318,16 +3318,16 @@
       </c>
       <c r="F12" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G12" s="13">
         <f t="shared" ref="G12:G35" ca="1" si="6">IF(F12="","",(D12-C12)-F12)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B13" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C13" s="3">
         <v>43171</v>
@@ -3341,11 +3341,11 @@
       </c>
       <c r="F13" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G13" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3549,11 +3549,11 @@
       </c>
       <c r="F22" s="13">
         <f ca="1">IF(((D22)=""),"",TODAY()-C22)</f>
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="G22" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3618,11 +3618,11 @@
       </c>
       <c r="F25" s="13">
         <f t="shared" ca="1" si="8"/>
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G25" s="13">
         <f t="shared" ref="G25:G28" ca="1" si="9">IF(F25="","",(D25-C25)-F25)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3641,11 +3641,11 @@
       </c>
       <c r="F26" s="13">
         <f t="shared" ca="1" si="8"/>
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G26" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3664,16 +3664,16 @@
       </c>
       <c r="F27" s="13">
         <f t="shared" ca="1" si="8"/>
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G27" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B28" s="14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C28" s="3">
         <v>43135</v>
@@ -3687,11 +3687,11 @@
       </c>
       <c r="F28" s="13">
         <f t="shared" ca="1" si="8"/>
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G28" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3710,16 +3710,16 @@
       </c>
       <c r="F29" s="13">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="G29" s="13">
         <f t="shared" ref="G29:G33" ca="1" si="11">IF(F29="","",(D29-C29)-F29)</f>
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B30" s="14" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C30" s="3">
         <v>43170</v>
@@ -3733,16 +3733,16 @@
       </c>
       <c r="F30" s="13">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G30" s="13">
         <f t="shared" ca="1" si="11"/>
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B31" s="14" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="C31" s="3">
         <v>43170</v>
@@ -3756,26 +3756,26 @@
       </c>
       <c r="F31" s="13">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G31" s="13">
         <f t="shared" ca="1" si="11"/>
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B32" s="14" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="C32" s="3">
-        <v>43170</v>
+        <v>43184</v>
       </c>
       <c r="D32" s="12">
         <f t="shared" si="10"/>
         <v>43198</v>
       </c>
       <c r="E32" s="6">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F32" s="13">
         <f t="shared" ca="1" si="8"/>
@@ -3783,22 +3783,22 @@
       </c>
       <c r="G32" s="13">
         <f t="shared" ca="1" si="11"/>
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B33" s="14" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="C33" s="3">
-        <v>43170</v>
+        <v>43184</v>
       </c>
       <c r="D33" s="12">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(E33),"",E33+C33)</f>
         <v>43198</v>
       </c>
       <c r="E33" s="6">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F33" s="13">
         <f t="shared" ca="1" si="8"/>
@@ -3806,7 +3806,7 @@
       </c>
       <c r="G33" s="13">
         <f t="shared" ca="1" si="11"/>
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3848,11 +3848,11 @@
       </c>
       <c r="F35" s="13">
         <f ca="1">IF(((D35)=""),"",TODAY()-C35)</f>
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="G35" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -3956,7 +3956,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.6">
       <c r="B19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.6">
@@ -4031,7 +4031,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B37" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.6">
@@ -4056,7 +4056,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.6">
       <c r="C43" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.6">
@@ -4226,57 +4226,57 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A79" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.6">
       <c r="B80" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B81" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B82" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A84" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B85" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B86" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B87" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.6">
       <c r="B88" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.6">
       <c r="C89" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.6">
       <c r="C90" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.6">
@@ -4306,12 +4306,12 @@
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.6">
       <c r="B98" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.6">
       <c r="B99" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
         <v>78</v>
@@ -4377,7 +4377,7 @@
         <v>26</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="19" t="s">
@@ -4386,17 +4386,17 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.6">
       <c r="G7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.6">
       <c r="G8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.6">
       <c r="G9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extension and Simulator Framework Update
Gantt update too.
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="129">
   <si>
     <t>Start Date</t>
   </si>
@@ -415,13 +415,7 @@
     <t>Extension: Simulator</t>
   </si>
   <si>
-    <t>Extension: M, A, F, D</t>
-  </si>
-  <si>
-    <t>(Optional) IEEE 754 Converter (Single, Double)</t>
-  </si>
-  <si>
-    <t>(Optional)  Extension Q &amp; Help Screen</t>
+    <t>Base: RV32I, RV64I; Extension: M, A, F, D</t>
   </si>
 </sst>
 </file>
@@ -712,9 +706,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Gantt Chart'!$B$5:$B$35</c:f>
+              <c:f>'Gantt Chart'!$B$5:$B$33</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>Capstone Project</c:v>
                 </c:pt>
@@ -749,16 +743,16 @@
                   <c:v>Phase III</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>Project Poster Draft</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Project Final Poster</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Poster Day</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>Project Final Report</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Project Poster Draft</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Project Final Poster</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Poster Day</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1 Minute Video</c:v>
@@ -794,18 +788,12 @@
                   <c:v>Extension: Simulator</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Extension: M, A, F, D</c:v>
+                  <c:v>Base: RV32I, RV64I; Extension: M, A, F, D</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>(Optional)  Extension Q &amp; Help Screen</c:v>
+                  <c:v>Final Integration &amp; Debugging</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>(Optional) IEEE 754 Converter (Single, Double)</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Final Integration &amp; Debugging</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>Capstone Project</c:v>
                 </c:pt>
               </c:strCache>
@@ -813,10 +801,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gantt Chart'!$C$5:$C$35</c:f>
+              <c:f>'Gantt Chart'!$C$5:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>43116</c:v>
                 </c:pt>
@@ -851,16 +839,16 @@
                   <c:v>43183</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43192</c:v>
+                  <c:v>43199</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43199</c:v>
+                  <c:v>43203</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43203</c:v>
+                  <c:v>43208</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43208</c:v>
+                  <c:v>43207</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>43214</c:v>
@@ -893,21 +881,15 @@
                   <c:v>43156</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43170</c:v>
+                  <c:v>43184</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43170</c:v>
+                  <c:v>43184</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43184</c:v>
+                  <c:v>43205</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43184</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>43184</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>43116</c:v>
                 </c:pt>
               </c:numCache>
@@ -1260,9 +1242,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Gantt Chart'!$B$5:$B$35</c:f>
+              <c:f>'Gantt Chart'!$B$5:$B$33</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>Capstone Project</c:v>
                 </c:pt>
@@ -1297,16 +1279,16 @@
                   <c:v>Phase III</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>Project Poster Draft</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Project Final Poster</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Poster Day</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>Project Final Report</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Project Poster Draft</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Project Final Poster</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Poster Day</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1 Minute Video</c:v>
@@ -1342,18 +1324,12 @@
                   <c:v>Extension: Simulator</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Extension: M, A, F, D</c:v>
+                  <c:v>Base: RV32I, RV64I; Extension: M, A, F, D</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>(Optional)  Extension Q &amp; Help Screen</c:v>
+                  <c:v>Final Integration &amp; Debugging</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>(Optional) IEEE 754 Converter (Single, Double)</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Final Integration &amp; Debugging</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>Capstone Project</c:v>
                 </c:pt>
               </c:strCache>
@@ -1361,12 +1337,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gantt Chart'!$F$5:$F$35</c:f>
+              <c:f>'Gantt Chart'!$F$5:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>27</c:v>
@@ -1384,19 +1360,19 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -1417,7 +1393,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>58</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>14</c:v>
@@ -1438,25 +1414,19 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>18</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>58</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1808,9 +1778,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Gantt Chart'!$B$5:$B$35</c:f>
+              <c:f>'Gantt Chart'!$B$5:$B$33</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>Capstone Project</c:v>
                 </c:pt>
@@ -1845,16 +1815,16 @@
                   <c:v>Phase III</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>Project Poster Draft</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Project Final Poster</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Poster Day</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>Project Final Report</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Project Poster Draft</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Project Final Poster</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Poster Day</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1 Minute Video</c:v>
@@ -1890,18 +1860,12 @@
                   <c:v>Extension: Simulator</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Extension: M, A, F, D</c:v>
+                  <c:v>Base: RV32I, RV64I; Extension: M, A, F, D</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>(Optional)  Extension Q &amp; Help Screen</c:v>
+                  <c:v>Final Integration &amp; Debugging</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>(Optional) IEEE 754 Converter (Single, Double)</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Final Integration &amp; Debugging</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>Capstone Project</c:v>
                 </c:pt>
               </c:strCache>
@@ -1909,12 +1873,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gantt Chart'!$G$5:$G$35</c:f>
+              <c:f>'Gantt Chart'!$G$5:$G$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>49</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1932,22 +1896,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>7</c:v>
@@ -1956,7 +1920,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>7</c:v>
@@ -1965,7 +1929,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>49</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -1986,25 +1950,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>49</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2742,7 +2700,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>64770</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3037,10 +2995,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:U35"/>
+  <dimension ref="B2:U33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -3156,11 +3114,11 @@
       </c>
       <c r="F5" s="13">
         <f ca="1">IF(((D5)=""),"",TODAY()-C5)</f>
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="G5" s="13">
         <f t="shared" ref="G5:G11" ca="1" si="0">IF(F5="","",(D5-C5)-F5)</f>
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3295,11 +3253,11 @@
       </c>
       <c r="F11" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G11" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3321,7 +3279,7 @@
         <v>14</v>
       </c>
       <c r="G12" s="13">
-        <f t="shared" ref="G12:G35" ca="1" si="6">IF(F12="","",(D12-C12)-F12)</f>
+        <f t="shared" ref="G12:G24" ca="1" si="6">IF(F12="","",(D12-C12)-F12)</f>
         <v>0</v>
       </c>
     </row>
@@ -3341,11 +3299,11 @@
       </c>
       <c r="F13" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G13" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3364,11 +3322,11 @@
       </c>
       <c r="F14" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G14" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
@@ -3387,26 +3345,26 @@
       </c>
       <c r="F15" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G15" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B16" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C16" s="3">
-        <v>43192</v>
+        <v>43199</v>
       </c>
       <c r="D16" s="12">
         <f t="shared" si="7"/>
         <v>43206</v>
       </c>
       <c r="E16" s="6">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F16" s="13">
         <f t="shared" ca="1" si="2"/>
@@ -3414,19 +3372,20 @@
       </c>
       <c r="G16" s="13">
         <f t="shared" ca="1" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B17" s="14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B17" s="14" t="s">
-        <v>11</v>
-      </c>
       <c r="C17" s="3">
-        <v>43199</v>
+        <v>43203</v>
       </c>
       <c r="D17" s="12">
         <f t="shared" si="7"/>
-        <v>43206</v>
+        <v>43210</v>
       </c>
       <c r="E17" s="6">
         <v>7</v>
@@ -3439,18 +3398,17 @@
         <f t="shared" ca="1" si="6"/>
         <v>7</v>
       </c>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+    </row>
+    <row r="18" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B18" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C18" s="3">
-        <v>43203</v>
+        <v>43208</v>
       </c>
       <c r="D18" s="12">
         <f t="shared" si="7"/>
-        <v>43210</v>
+        <v>43215</v>
       </c>
       <c r="E18" s="6">
         <v>7</v>
@@ -3464,30 +3422,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="19" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B19" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" s="3">
-        <v>43208</v>
+        <v>43207</v>
       </c>
       <c r="D19" s="12">
-        <f t="shared" si="7"/>
-        <v>43215</v>
+        <f t="shared" ref="D19" si="8">IF(ISBLANK(E19),"",E19+C19)</f>
+        <v>43221</v>
       </c>
       <c r="E19" s="6">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F19" s="13">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ref="F19" ca="1" si="9">IF(((D19)=""),"",IF(TODAY()&lt;C19,0,IF(TODAY()&lt;D19,TODAY()-C19,E19)))</f>
         <v>0</v>
       </c>
       <c r="G19" s="13">
-        <f t="shared" ca="1" si="6"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+        <f t="shared" ref="G19" ca="1" si="10">IF(F19="","",(D19-C19)-F19)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B20" s="14" t="s">
         <v>16</v>
       </c>
@@ -3510,7 +3468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="21" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B21" s="14" t="s">
         <v>17</v>
       </c>
@@ -3533,7 +3491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B22" s="20" t="s">
         <v>8</v>
       </c>
@@ -3549,14 +3507,14 @@
       </c>
       <c r="F22" s="13">
         <f ca="1">IF(((D22)=""),"",TODAY()-C22)</f>
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="G22" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B23" s="14" t="s">
         <v>65</v>
       </c>
@@ -3571,7 +3529,7 @@
         <v>14</v>
       </c>
       <c r="F23" s="13">
-        <f t="shared" ref="F23:F34" ca="1" si="8">IF(((D23)=""),"",IF(TODAY()&lt;C23,0,IF(TODAY()&lt;D23,TODAY()-C23,E23)))</f>
+        <f t="shared" ref="F23:F31" ca="1" si="11">IF(((D23)=""),"",IF(TODAY()&lt;C23,0,IF(TODAY()&lt;D23,TODAY()-C23,E23)))</f>
         <v>14</v>
       </c>
       <c r="G23" s="13">
@@ -3579,7 +3537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="24" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B24" s="14" t="s">
         <v>30</v>
       </c>
@@ -3594,7 +3552,7 @@
         <v>7</v>
       </c>
       <c r="F24" s="13">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="11"/>
         <v>7</v>
       </c>
       <c r="G24" s="13">
@@ -3602,7 +3560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="25" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B25" s="14" t="s">
         <v>78</v>
       </c>
@@ -3617,15 +3575,15 @@
         <v>28</v>
       </c>
       <c r="F25" s="13">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="11"/>
         <v>28</v>
       </c>
       <c r="G25" s="13">
-        <f t="shared" ref="G25:G28" ca="1" si="9">IF(F25="","",(D25-C25)-F25)</f>
+        <f t="shared" ref="G25:G28" ca="1" si="12">IF(F25="","",(D25-C25)-F25)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="26" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B26" s="14" t="s">
         <v>101</v>
       </c>
@@ -3640,15 +3598,15 @@
         <v>28</v>
       </c>
       <c r="F26" s="13">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="11"/>
         <v>28</v>
       </c>
       <c r="G26" s="13">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="27" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B27" s="14" t="s">
         <v>26</v>
       </c>
@@ -3656,22 +3614,22 @@
         <v>43135</v>
       </c>
       <c r="D27" s="12">
-        <f t="shared" ref="D27:D34" si="10">IF(ISBLANK(E27),"",E27+C27)</f>
+        <f t="shared" ref="D27:D31" si="13">IF(ISBLANK(E27),"",E27+C27)</f>
         <v>43163</v>
       </c>
       <c r="E27" s="6">
         <v>28</v>
       </c>
       <c r="F27" s="13">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="11"/>
         <v>28</v>
       </c>
       <c r="G27" s="13">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="28" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B28" s="14" t="s">
         <v>118</v>
       </c>
@@ -3679,22 +3637,22 @@
         <v>43135</v>
       </c>
       <c r="D28" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>43163</v>
       </c>
       <c r="E28" s="6">
         <v>28</v>
       </c>
       <c r="F28" s="13">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="11"/>
         <v>28</v>
       </c>
       <c r="G28" s="13">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="29" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B29" s="14" t="s">
         <v>102</v>
       </c>
@@ -3702,157 +3660,111 @@
         <v>43156</v>
       </c>
       <c r="D29" s="12">
-        <f t="shared" si="10"/>
-        <v>43177</v>
+        <f t="shared" si="13"/>
+        <v>43191</v>
       </c>
       <c r="E29" s="6">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F29" s="13">
-        <f t="shared" ca="1" si="8"/>
-        <v>18</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>31</v>
       </c>
       <c r="G29" s="13">
-        <f t="shared" ref="G29:G33" ca="1" si="11">IF(F29="","",(D29-C29)-F29)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+        <f t="shared" ref="G29:G31" ca="1" si="14">IF(F29="","",(D29-C29)-F29)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B30" s="14" t="s">
         <v>127</v>
       </c>
       <c r="C30" s="3">
-        <v>43170</v>
+        <v>43184</v>
       </c>
       <c r="D30" s="12">
-        <f t="shared" si="10"/>
-        <v>43198</v>
+        <f t="shared" si="13"/>
+        <v>43212</v>
       </c>
       <c r="E30" s="6">
         <v>28</v>
       </c>
       <c r="F30" s="13">
-        <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>3</v>
       </c>
       <c r="G30" s="13">
-        <f t="shared" ca="1" si="11"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+        <f t="shared" ca="1" si="14"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B31" s="14" t="s">
         <v>128</v>
       </c>
       <c r="C31" s="3">
-        <v>43170</v>
+        <v>43184</v>
       </c>
       <c r="D31" s="12">
-        <f t="shared" si="10"/>
-        <v>43198</v>
+        <f t="shared" si="13"/>
+        <v>43212</v>
       </c>
       <c r="E31" s="6">
         <v>28</v>
       </c>
       <c r="F31" s="13">
-        <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>3</v>
       </c>
       <c r="G31" s="13">
-        <f t="shared" ca="1" si="11"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.6">
+        <f t="shared" ca="1" si="14"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B32" s="14" t="s">
-        <v>130</v>
+        <v>21</v>
       </c>
       <c r="C32" s="3">
-        <v>43184</v>
+        <v>43205</v>
       </c>
       <c r="D32" s="12">
-        <f t="shared" si="10"/>
-        <v>43198</v>
+        <f>IF(ISBLANK(E32),"",E32+C32)</f>
+        <v>43220</v>
       </c>
       <c r="E32" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F32" s="13">
-        <f t="shared" ca="1" si="8"/>
+        <f ca="1">IF(((D32)=""),"",IF(TODAY()&lt;C32,0,IF(TODAY()&lt;D32,TODAY()-C32,E32)))</f>
         <v>0</v>
       </c>
       <c r="G32" s="13">
-        <f t="shared" ca="1" si="11"/>
-        <v>14</v>
+        <f ca="1">IF(F32="","",(D32-C32)-F32)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B33" s="14" t="s">
-        <v>129</v>
+      <c r="B33" s="20" t="s">
+        <v>8</v>
       </c>
       <c r="C33" s="3">
-        <v>43184</v>
+        <v>43116</v>
       </c>
       <c r="D33" s="12">
         <f>IF(ISBLANK(E33),"",E33+C33)</f>
-        <v>43198</v>
+        <v>43223</v>
       </c>
       <c r="E33" s="6">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="F33" s="13">
-        <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <f ca="1">IF(((D33)=""),"",TODAY()-C33)</f>
+        <v>71</v>
       </c>
       <c r="G33" s="13">
-        <f t="shared" ca="1" si="11"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B34" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="3">
-        <v>43184</v>
-      </c>
-      <c r="D34" s="12">
-        <f t="shared" si="10"/>
-        <v>43205</v>
-      </c>
-      <c r="E34" s="6">
-        <v>21</v>
-      </c>
-      <c r="F34" s="13">
-        <f t="shared" ca="1" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G34" s="13">
-        <f t="shared" ca="1" si="6"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B35" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="3">
-        <v>43116</v>
-      </c>
-      <c r="D35" s="12">
-        <f>IF(ISBLANK(E35),"",E35+C35)</f>
-        <v>43223</v>
-      </c>
-      <c r="E35" s="6">
-        <v>107</v>
-      </c>
-      <c r="F35" s="13">
-        <f ca="1">IF(((D35)=""),"",TODAY()-C35)</f>
-        <v>58</v>
-      </c>
-      <c r="G35" s="13">
-        <f t="shared" ca="1" si="6"/>
-        <v>49</v>
+        <f ca="1">IF(F33="","",(D33-C33)-F33)</f>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>